<commit_message>
commit after adding retry and takescreenshot
</commit_message>
<xml_diff>
--- a/7rmart_supermarket/src/main/resources/TestData.xlsx
+++ b/7rmart_supermarket/src/main/resources/TestData.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\7rMart\7rmart_supermarket\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF74DC-0766-41FF-8F46-9E741196A6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014F3BD4-4403-449B-AA0E-6E92385618D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="762" activeTab="1" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="9" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="ManageSliderPage" sheetId="10" r:id="rId2"/>
     <sheet name="AdminUsersPage" sheetId="5" r:id="rId3"/>
-    <sheet name="AddLocationsPage" sheetId="4" r:id="rId4"/>
-    <sheet name="ManageDeliveryBoyPage" sheetId="2" r:id="rId5"/>
-    <sheet name="MenuPage" sheetId="3" r:id="rId6"/>
-    <sheet name="ManageOfferCodePage" sheetId="6" r:id="rId7"/>
-    <sheet name="ManageOrdersPage" sheetId="9" r:id="rId8"/>
-    <sheet name="MobileSliderPage" sheetId="7" r:id="rId9"/>
+    <sheet name="PushNotificationPage" sheetId="11" r:id="rId4"/>
+    <sheet name="AddLocationsPage" sheetId="4" r:id="rId5"/>
+    <sheet name="ManageDeliveryBoyPage" sheetId="2" r:id="rId6"/>
+    <sheet name="MenuPage" sheetId="3" r:id="rId7"/>
+    <sheet name="ManageOfferCodePage" sheetId="6" r:id="rId8"/>
+    <sheet name="ManageOrdersPage" sheetId="9" r:id="rId9"/>
+    <sheet name="MobileSliderPage" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>CorrectUsername</t>
   </si>
@@ -193,22 +194,94 @@
     <t>Order Id</t>
   </si>
   <si>
-    <t>� 
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https//:hshcxgcjshfcjshcjh</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Good Morning</t>
+  </si>
+  <si>
+    <t>This is a message for users</t>
+  </si>
+  <si>
+    <t>×
+Alert!
+Message send successfully</t>
+  </si>
+  <si>
+    <t>Page Heading</t>
+  </si>
+  <si>
+    <t>List Pages</t>
+  </si>
+  <si>
+    <t>List Categories</t>
+  </si>
+  <si>
+    <t>List Products</t>
+  </si>
+  <si>
+    <t>List Offercodes</t>
+  </si>
+  <si>
+    <t>List Sliders</t>
+  </si>
+  <si>
+    <t>List Delivery Boy</t>
+  </si>
+  <si>
+    <t>List Users</t>
+  </si>
+  <si>
+    <t>List Orders</t>
+  </si>
+  <si>
+    <t>List Locations</t>
+  </si>
+  <si>
+    <t>List Mobile Sliders</t>
+  </si>
+  <si>
+    <t>List Expense</t>
+  </si>
+  <si>
+    <t>Time Field 1</t>
+  </si>
+  <si>
+    <t>10:00am</t>
+  </si>
+  <si>
+    <t>Time Field 2</t>
+  </si>
+  <si>
+    <t>6:30pm</t>
+  </si>
+  <si>
+    <t>Expected Text</t>
+  </si>
+  <si>
+    <t>01-Jan-1970
+05:00pm to 10:00pm</t>
+  </si>
+  <si>
+    <t>�
 Alert!
 Mobile Slider Created Successfully</t>
   </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>https//:hshcxgcjshfcjshcjh</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +303,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -258,11 +344,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -628,11 +719,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F57B712-431E-4372-9D28-D6570D5EA924}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DC58E6-634E-41D3-86B8-427ECB8F2B0D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -643,12 +769,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -698,6 +824,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BEE7F7-59A1-4CFA-A78D-A12B191CBD89}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B62EDA-173E-4F8F-869D-DFE81A91670C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -748,7 +917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439101D6-ADD1-4E6A-850A-7F382DC4245C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -789,93 +958,138 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA7BE15-D606-4F7D-89E4-33DCF83F8866}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -890,7 +1104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38E6722-9D56-470F-AC29-9A972981A052}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -941,92 +1155,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36218722-09FB-4B1B-BC92-7F4D879DA99D}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F57B712-431E-4372-9D28-D6570D5EA924}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit after adding new TestNG files
</commit_message>
<xml_diff>
--- a/7rmart_supermarket/src/main/resources/TestData.xlsx
+++ b/7rmart_supermarket/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\7rMart\7rmart_supermarket\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014F3BD4-4403-449B-AA0E-6E92385618D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21727C6-75FC-468A-B981-CE0B0F93BC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="9" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="8" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -723,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F57B712-431E-4372-9D28-D6570D5EA924}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
@@ -1159,12 +1159,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36218722-09FB-4B1B-BC92-7F4D879DA99D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
@@ -1186,7 +1187,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>69</v>
@@ -1200,37 +1201,37 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit after minor Changes
</commit_message>
<xml_diff>
--- a/7rmart_supermarket/src/main/resources/TestData.xlsx
+++ b/7rmart_supermarket/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\7rMart\7rmart_supermarket\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21727C6-75FC-468A-B981-CE0B0F93BC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF0B28B-3E81-4E27-A12A-268B3CBD3D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2460" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="8" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="7" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Expected Alert Message</t>
   </si>
   <si>
-    <t>FIRST25</t>
-  </si>
-  <si>
     <t>×
 Alert!
 Offer Created Successfully</t>
@@ -275,6 +272,9 @@
     <t>�
 Alert!
 Mobile Slider Created Successfully</t>
+  </si>
+  <si>
+    <t>FIRST30</t>
   </si>
 </sst>
 </file>
@@ -735,10 +735,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -769,12 +769,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -839,18 +839,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="56.25" x14ac:dyDescent="0.3">
@@ -858,7 +858,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +977,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,14 +1108,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38E6722-9D56-470F-AC29-9A972981A052}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1125,7 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,7 +1133,7 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1149,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36218722-09FB-4B1B-BC92-7F4D879DA99D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1173,16 +1175,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1190,13 +1192,13 @@
         <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit after error correction
</commit_message>
<xml_diff>
--- a/7rmart_supermarket/src/main/resources/TestData.xlsx
+++ b/7rmart_supermarket/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\7rMart\7rmart_supermarket\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF0B28B-3E81-4E27-A12A-268B3CBD3D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E006E84B-5721-4EFD-90FD-3426A3162D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2460" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="7" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="21600" windowHeight="11835" tabRatio="762" firstSheet="7" activeTab="8" xr2:uid="{C805B247-64AB-4589-A923-860AF548A4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>CorrectUsername</t>
   </si>
@@ -248,25 +248,6 @@
   </si>
   <si>
     <t>List Expense</t>
-  </si>
-  <si>
-    <t>Time Field 1</t>
-  </si>
-  <si>
-    <t>10:00am</t>
-  </si>
-  <si>
-    <t>Time Field 2</t>
-  </si>
-  <si>
-    <t>6:30pm</t>
-  </si>
-  <si>
-    <t>Expected Text</t>
-  </si>
-  <si>
-    <t>01-Jan-1970
-05:00pm to 10:00pm</t>
   </si>
   <si>
     <t>�
@@ -746,7 +727,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1108,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38E6722-9D56-470F-AC29-9A972981A052}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1125,7 +1106,7 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36218722-09FB-4B1B-BC92-7F4D879DA99D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1177,63 +1158,48 @@
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>145</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>72</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>